<commit_message>
Versão Final do Anal. Sint. - relatório pendente
</commit_message>
<xml_diff>
--- a/TabelaParser.xlsx
+++ b/TabelaParser.xlsx
@@ -786,7 +786,7 @@
   <dimension ref="A1:AH32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -811,7 +811,7 @@
     <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="3.83203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4.6640625" customWidth="1"/>
-    <col min="24" max="24" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="3.83203125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="4.5" customWidth="1"/>
     <col min="26" max="26" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="3.83203125" bestFit="1" customWidth="1"/>

</xml_diff>